<commit_message>
form 변경 to hair
</commit_message>
<xml_diff>
--- a/dailyreport_form.xlsx
+++ b/dailyreport_form.xlsx
@@ -162,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -199,47 +199,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -274,13 +233,133 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -302,34 +381,58 @@
     <xf numFmtId="21" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -649,7 +752,7 @@
   <dimension ref="A1:AC32"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -667,15 +770,15 @@
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12">
+      <c r="B1" s="10">
         <v>43800</v>
       </c>
-      <c r="C1" s="13"/>
+      <c r="C1" s="11"/>
       <c r="H1" s="1"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
@@ -688,183 +791,183 @@
       <c r="AC1" s="2"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14" t="s">
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14" t="s">
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14" t="s">
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14" t="s">
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14" t="s">
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14" t="s">
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
     </row>
     <row r="3" spans="1:29" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="P3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="R3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="S3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="T3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="U3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="V3" s="10" t="s">
+      <c r="V3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c r="W3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="X3" s="10" t="s">
+      <c r="X3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="10" t="s">
+      <c r="Y3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Z3" s="10" t="s">
+      <c r="Z3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AA3" s="10" t="s">
+      <c r="AA3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" s="10" t="s">
+      <c r="AB3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AC3" s="10" t="s">
+      <c r="AC3" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="8"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="16"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="11"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -887,15 +990,15 @@
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
       <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
+      <c r="AC5" s="19"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="11"/>
+      <c r="F6" s="18"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -918,15 +1021,15 @@
       <c r="Z6" s="6"/>
       <c r="AA6" s="6"/>
       <c r="AB6" s="6"/>
-      <c r="AC6" s="6"/>
+      <c r="AC6" s="19"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="11"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -949,15 +1052,15 @@
       <c r="Z7" s="6"/>
       <c r="AA7" s="6"/>
       <c r="AB7" s="6"/>
-      <c r="AC7" s="6"/>
+      <c r="AC7" s="19"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="11"/>
+      <c r="F8" s="18"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -980,15 +1083,15 @@
       <c r="Z8" s="6"/>
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
-      <c r="AC8" s="6"/>
+      <c r="AC8" s="19"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="11"/>
+      <c r="F9" s="18"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -1011,15 +1114,15 @@
       <c r="Z9" s="6"/>
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
-      <c r="AC9" s="6"/>
+      <c r="AC9" s="19"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="11"/>
+      <c r="F10" s="18"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -1042,15 +1145,15 @@
       <c r="Z10" s="6"/>
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
-      <c r="AC10" s="6"/>
+      <c r="AC10" s="19"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="11"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -1073,15 +1176,15 @@
       <c r="Z11" s="6"/>
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
-      <c r="AC11" s="6"/>
+      <c r="AC11" s="19"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="11"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -1104,15 +1207,15 @@
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
-      <c r="AC12" s="6"/>
+      <c r="AC12" s="19"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="11"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -1135,15 +1238,15 @@
       <c r="Z13" s="6"/>
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
-      <c r="AC13" s="6"/>
+      <c r="AC13" s="19"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="11"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -1166,15 +1269,15 @@
       <c r="Z14" s="6"/>
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
+      <c r="AC14" s="19"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="11"/>
+      <c r="F15" s="18"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -1197,15 +1300,15 @@
       <c r="Z15" s="6"/>
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
-      <c r="AC15" s="6"/>
+      <c r="AC15" s="19"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="11"/>
+      <c r="F16" s="18"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -1228,15 +1331,15 @@
       <c r="Z16" s="6"/>
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
-      <c r="AC16" s="6"/>
+      <c r="AC16" s="19"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="18"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -1259,15 +1362,15 @@
       <c r="Z17" s="6"/>
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
-      <c r="AC17" s="6"/>
+      <c r="AC17" s="19"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="11"/>
+      <c r="F18" s="18"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -1290,15 +1393,15 @@
       <c r="Z18" s="6"/>
       <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
-      <c r="AC18" s="6"/>
+      <c r="AC18" s="19"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="11"/>
+      <c r="F19" s="18"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -1321,15 +1424,15 @@
       <c r="Z19" s="6"/>
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
-      <c r="AC19" s="6"/>
+      <c r="AC19" s="19"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
-      <c r="F20" s="11"/>
+      <c r="F20" s="18"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -1352,15 +1455,15 @@
       <c r="Z20" s="6"/>
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
-      <c r="AC20" s="6"/>
+      <c r="AC20" s="19"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="11"/>
+      <c r="F21" s="18"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -1383,15 +1486,15 @@
       <c r="Z21" s="6"/>
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
-      <c r="AC21" s="6"/>
+      <c r="AC21" s="19"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="11"/>
+      <c r="F22" s="18"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -1414,15 +1517,15 @@
       <c r="Z22" s="6"/>
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
-      <c r="AC22" s="6"/>
+      <c r="AC22" s="19"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="11"/>
+      <c r="F23" s="18"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -1445,15 +1548,15 @@
       <c r="Z23" s="6"/>
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
-      <c r="AC23" s="6"/>
+      <c r="AC23" s="19"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="11"/>
+      <c r="F24" s="18"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -1476,15 +1579,15 @@
       <c r="Z24" s="6"/>
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
-      <c r="AC24" s="6"/>
+      <c r="AC24" s="19"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="11"/>
+      <c r="F25" s="18"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -1507,15 +1610,15 @@
       <c r="Z25" s="6"/>
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
-      <c r="AC25" s="6"/>
+      <c r="AC25" s="19"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
-      <c r="F26" s="11"/>
+      <c r="F26" s="18"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -1538,38 +1641,38 @@
       <c r="Z26" s="6"/>
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
-      <c r="AC26" s="6"/>
+      <c r="AC26" s="19"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
-      <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
-      <c r="W27" s="6"/>
-      <c r="X27" s="6"/>
-      <c r="Y27" s="6"/>
-      <c r="Z27" s="6"/>
-      <c r="AA27" s="6"/>
-      <c r="AB27" s="6"/>
-      <c r="AC27" s="6"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="22"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="22"/>
+      <c r="Y27" s="22"/>
+      <c r="Z27" s="22"/>
+      <c r="AA27" s="22"/>
+      <c r="AB27" s="22"/>
+      <c r="AC27" s="24"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="F28" s="4"/>
@@ -1617,11 +1720,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="R1:S1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="O2:Q2"/>
@@ -1630,6 +1728,11 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:K2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="AA2:AC2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="R1:S1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>